<commit_message>
latesr run log and downloaded_excels
</commit_message>
<xml_diff>
--- a/docs/uc_page_htmls/downloaded_excels/UC567-base_order_info.xlsx
+++ b/docs/uc_page_htmls/downloaded_excels/UC567-base_order_info.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,32 +491,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>UC567-1186</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>02 Jan 2026, 07:22 PM</t>
+          <t>UC567-1318</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>31 Jan 2026, 01:54 PM</t>
+          <t>31 Jan 2026, 02:07 PM</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ganeshm</t>
+          <t>GORAV SINGH</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>9384856438</t>
+          <t>8750000835</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>C Dot Apartment, A-801, Sector-56, Ghata , Near sushant lok tower</t>
+          <t>SHUSHANT TOWER 7 TH FLOOR, , ,</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -531,7 +526,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>APP</t>
+          <t>WALK-IN</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -541,7 +536,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>31 Jan 2026, 01:54 PM</t>
+          <t>31 Jan 2026, 02:07 PM</t>
         </is>
       </c>
     </row>
@@ -553,17 +548,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>UC567-1289</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>24 Jan 2026, 04:25 PM</t>
+          <t>UC567-1132</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>31 Jan 2026, 01:53 PM</t>
+          <t>31 Jan 2026, 01:56 PM</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -593,7 +583,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>APP</t>
+          <t>WALK-IN</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -603,7 +593,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>31 Jan 2026, 01:53 PM</t>
+          <t>31 Jan 2026, 01:56 PM</t>
         </is>
       </c>
     </row>
@@ -615,32 +605,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>UC567-1293</t>
+          <t>UC567-1186</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>25 Jan 2026, 12:01 PM</t>
+          <t>02 Jan 2026, 07:22 PM</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>27 Jan 2026, 07:24 PM</t>
+          <t>31 Jan 2026, 01:54 PM</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Mr Pavan</t>
+          <t>ganeshm</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>9990859908</t>
+          <t>9384856438</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Flat 2 D jnu aravali apartment, , Sector 56,</t>
+          <t>C Dot Apartment, A-801, Sector-56, Ghata , Near sushant lok tower</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -655,7 +645,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>UCLEAN STORE</t>
+          <t>APP</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -665,7 +655,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>27 Jan 2026, 07:24 PM</t>
+          <t>31 Jan 2026, 01:54 PM</t>
         </is>
       </c>
     </row>
@@ -677,57 +667,1207 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>UC567-1289</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>24 Jan 2026, 04:25 PM</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>31 Jan 2026, 01:53 PM</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ganeshm</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>9384856438</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>C Dot Apartment, A-801, Sector-56, Ghata , Near sushant lok tower</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>APP</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>31 Jan 2026, 01:53 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>UC567-1312</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>31 Jan 2026, 01:20 PM</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Anmol Garg</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>9999472151</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Flat no 124 tower no 6 , Hewo apartments part 1 , Behind rail vihar</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>31 Jan 2026, 01:20 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>UC567-1277</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>31 Jan 2026, 12:21 PM</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>NAGESH</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>8306782240</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>house E 197 E block, , sushat lok 2,</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>31 Jan 2026, 12:21 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>UC567-1320</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>30 Jan 2026, 02:02 PM</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Tusher Garg</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>9828609562</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>12, Hindustan Road, , ,</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Payment Pending</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>30 Jan 2026, 02:02 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>UC567-1240</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>30 Jan 2026, 12:05 PM</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Ms Ritu</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>8448489869</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>B 3 - 501, Exotica, , ,</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>30 Jan 2026, 12:05 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>UC567-1293</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>25 Jan 2026, 12:01 PM</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>27 Jan 2026, 07:24 PM</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Mr Pavan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>9990859908</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Flat 2 D jnu aravali apartment, , Sector 56,</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>UCLEAN STORE</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>27 Jan 2026, 07:24 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>UC567-1279</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>26 Jan 2026, 12:20 PM</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Manoj Bhati</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>7357515575</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>D170 Sl-2, , sec 56,</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>26 Jan 2026, 12:20 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>UC567-1292</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>25 Jan 2026, 03:29 PM</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>AMMAN VOHRA</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>9999894294</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>C-37 SUSHANT LOK 2 SECTOR 56 GURGAON , , ,</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>25 Jan 2026, 03:29 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>UC567-1276</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>22 Jan 2026, 12:15 PM</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>mohit saloon</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>8851999375</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>shop , , 2, sushant tower</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>22 Jan 2026, 12:15 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>UC567-1268</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>18 Jan 2026, 08:29 PM</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>21 Jan 2026, 06:08 PM</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>Mr Sohum</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>8459413171</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>C 73, 303, 3rd floor, , ,</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>View Payment Details</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Handle with care</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
         <is>
           <t>UCLEAN STORE</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Delivered</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
         <is>
           <t>21 Jan 2026, 06:08 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>UC567-1271</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>21 Jan 2026, 11:54 AM</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>R B Tiwari</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>9650180228</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Sushant Tower, , Sec 56,</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>21 Jan 2026, 11:54 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>UC567-1274</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>21 Jan 2026, 11:54 AM</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>R B Tiwari</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>9650180228</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Sushant Tower, , Sec 56,</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>21 Jan 2026, 11:54 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>UC567-1264</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>19 Jan 2026, 07:03 PM</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Tushar</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>9828609862</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>sec56 , , ,</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>19 Jan 2026, 07:03 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>UC567-1247</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>18 Jan 2026, 08:27 PM</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>sanjeev</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>9663455660</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Cdot, , Appartment , sec 56</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>18 Jan 2026, 08:27 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>UC567-1257</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>18 Jan 2026, 05:50 PM</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>mohit saloon</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>8851999375</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>shop , , 2, sushant tower</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>18 Jan 2026, 05:50 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>UC567-1236</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>18 Jan 2026, 03:10 PM</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Mr. Vikas</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>9899107469</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>D1/41 Rosewood City Sector 49, , Gurugram,</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>18 Jan 2026, 03:10 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>UC567-1147</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>18 Jan 2026, 02:44 PM</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>PUJA</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>9312567990</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>G -106 A SHUSHANT LOK -2 SECTOR 56, , ,</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>18 Jan 2026, 02:44 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>UC567-1242</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>18 Jan 2026, 01:35 PM</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Dhuruv</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>9650125788</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Sec 56, , ,</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>18 Jan 2026, 01:35 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>UC567-1239</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>17 Jan 2026, 07:52 PM</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>HARPREET</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>9999914674</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>H.NO- 307 3RD FLOOR, , SHUSHANT TOWER,</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>17 Jan 2026, 07:52 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>UC567-1243</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>17 Jan 2026, 07:52 PM</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>HARPREET</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>9999914674</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>H.NO- 307 3RD FLOOR, , SHUSHANT TOWER,</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>17 Jan 2026, 07:52 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>UC567</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>UC567-1198</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>17 Jan 2026, 03:13 PM</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Mr Kumar Lokesh</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>9801839332</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>D 184 GF Sushant lok 2, , Sector 56,</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>View Payment Details</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Handle with care</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>WALK-IN</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>17 Jan 2026, 03:13 PM</t>
         </is>
       </c>
     </row>

</xml_diff>